<commit_message>
Adding approach is in progress
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -5,19 +5,22 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ahmer Saeed\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\zabbix_custom\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8904" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8904" firstSheet="5" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Wordpress Site" sheetId="1" r:id="rId1"/>
     <sheet name="Shopify Site" sheetId="2" r:id="rId2"/>
     <sheet name="Raw Dev - Business Site" sheetId="3" r:id="rId3"/>
-    <sheet name="Sheet7" sheetId="7" r:id="rId4"/>
-    <sheet name="Raw Dev - Ecomm Site" sheetId="5" r:id="rId5"/>
-    <sheet name="Raw Dev - Site Architecture" sheetId="6" r:id="rId6"/>
+    <sheet name="Raw Dev - Ecom Site" sheetId="5" r:id="rId4"/>
+    <sheet name="Raw Dev Busines Site - Approach" sheetId="6" r:id="rId5"/>
+    <sheet name="Raw Dev Ecomm Site - Approach" sheetId="10" r:id="rId6"/>
+    <sheet name="Task List" sheetId="7" r:id="rId7"/>
+    <sheet name="Sheet2" sheetId="9" r:id="rId8"/>
+    <sheet name="InertiaSft Repo Site - Approach" sheetId="8" r:id="rId9"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -29,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="104">
   <si>
     <t>Check efficient way of deploying Wordpress site on different env</t>
   </si>
@@ -55,9 +58,6 @@
     <t>Create Website structure on React which contains Home, About Us, Products, Blogs, Carrier and Contact Us Pages</t>
   </si>
   <si>
-    <t>Maintaine repo of pre-built Sliders, Nav Bar, Forms, Email subscriber section, Video Player Image, Blogs grid</t>
-  </si>
-  <si>
     <t>What if, we can make it dynamic as well saving structure in db and render it as per the request</t>
   </si>
   <si>
@@ -223,9 +223,6 @@
     <t>Medium Level</t>
   </si>
   <si>
-    <t>With all the capabilities of Medium Level what if, if we save the entire html, css of our raw dev structure in the schema as well and assigning it types</t>
-  </si>
-  <si>
     <t>Each structure will know what re-usable components APIs should it call</t>
   </si>
   <si>
@@ -244,18 +241,9 @@
     <t>Fast performance APIs will be built to achieve this also passing data between back-end and front-end should not disturb the html and css of these re-usable components</t>
   </si>
   <si>
-    <t>We should Cache techniques to enhance the performance of binding re-usable components to front-end from back-end</t>
-  </si>
-  <si>
     <t>APIs should take structure name or identifer in order to differentiate them while binding the re-usable components</t>
   </si>
   <si>
-    <t>Use npm install like command to set the re-usable components only once without calling APIs everytime</t>
-  </si>
-  <si>
-    <t>CSS files should be contain by the structure file, re-usable components saved inside mongo will only contain the class and ids</t>
-  </si>
-  <si>
     <t>To save the content of each re-usable components w.r.t customer will be handle by creating and configuring customer's own database. For now (this MVP) we will add content using insert scripts</t>
   </si>
   <si>
@@ -284,6 +272,78 @@
   </si>
   <si>
     <t>Create build and deploy all the components (front-end,back-end and db) it on QA server to Test (both front-end and back-end i-e NodeJS)</t>
+  </si>
+  <si>
+    <t>CSS files should be contain by the structure it self, re-usable components saved inside mongo will only contain the class and ids</t>
+  </si>
+  <si>
+    <t>Sit with asjad to check the injection of re-usable components</t>
+  </si>
+  <si>
+    <t>Ask management to list the re-usable component we will provide</t>
+  </si>
+  <si>
+    <t>Ask management to share the theme idea for wordpress business site, ecommerce site, raw dev business site, raw ecommerce site</t>
+  </si>
+  <si>
+    <t>Providing hosting machines to create enviornments.</t>
+  </si>
+  <si>
+    <t>Nav Bars</t>
+  </si>
+  <si>
+    <t>https://www.mockplus.com/blog/post/bootstrap-navbar-template</t>
+  </si>
+  <si>
+    <t>Approach 1</t>
+  </si>
+  <si>
+    <t>For Demo site Contact Us Forms, Login Signup Forms should be handle in a sense that It will not call APIs</t>
+  </si>
+  <si>
+    <t>We should use cache techniques to enhance the performance of binding re-usable components to front-end from back-end</t>
+  </si>
+  <si>
+    <t>Approach 2</t>
+  </si>
+  <si>
+    <t>For this we have to manage the identification of re-usable components by developing custom logic</t>
+  </si>
+  <si>
+    <t>Re-usable components will contain html and css classes or may be css files as well. For this part we have two options either putting css files of re-usable components along with structure files, Secondly we should put css files of re-usable components along with the re-usable components.</t>
+  </si>
+  <si>
+    <t>For this we will add content in the re-usable component after adding them using the npm install command</t>
+  </si>
+  <si>
+    <t>We will use github repository and npm plugin to store and organize the re-usable components files. This will help in adding re-usable compnents to our pre-built structure by executing npm install commands. This addition will be once at a time no need to get re-usable components everytime via API calls.</t>
+  </si>
+  <si>
+    <t>Approach-1 or Approach 2 of adding re-usable components</t>
+  </si>
+  <si>
+    <t>With all the capabilities of Medium Level Approach 1 what if, if we save the entire html, css of our raw dev structure in the schema as well and assigning it types</t>
+  </si>
+  <si>
+    <t>This will help in avoiding node server if website has no requirement of dynamic site</t>
+  </si>
+  <si>
+    <t>Approach</t>
+  </si>
+  <si>
+    <t>Make use of code base of Vendure to build the basic ecommerce project</t>
+  </si>
+  <si>
+    <t>Search for re-usable components (plagirism and copyright should be consider)</t>
+  </si>
+  <si>
+    <t>Execute approach 1 or 2 in order to adding the re-usable components</t>
+  </si>
+  <si>
+    <t>Create structure similarly as in Raw Dev Business Site</t>
+  </si>
+  <si>
+    <t>Execute Approach 1 or 2</t>
   </si>
 </sst>
 </file>
@@ -299,8 +359,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -329,8 +390,9 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -365,11 +427,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -669,27 +730,27 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.3">
@@ -704,7 +765,7 @@
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.3">
@@ -714,62 +775,62 @@
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -781,7 +842,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
@@ -800,27 +861,27 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.3">
@@ -835,7 +896,7 @@
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.3">
@@ -845,62 +906,62 @@
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -910,10 +971,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B25"/>
+  <dimension ref="A1:B22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -924,7 +985,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -934,12 +995,12 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
@@ -947,100 +1008,85 @@
         <v>7</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>78</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" s="12" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" s="12" t="s">
-        <v>11</v>
+      <c r="A10" s="2" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" s="2" t="s">
-        <v>16</v>
+      <c r="A12" s="7" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A15" s="7" t="s">
-        <v>18</v>
+      <c r="A15" s="2" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
-        <v>82</v>
+        <v>79</v>
+      </c>
+      <c r="B18" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
-        <v>83</v>
+        <v>51</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A20" s="12" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A21" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="B21" t="s">
-        <v>13</v>
+      <c r="A20" s="2" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A22" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A23" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A25" s="7" t="s">
-        <v>31</v>
+      <c r="A22" s="7" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -1051,43 +1097,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="33.109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>81</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B21"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1098,7 +1111,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -1108,98 +1121,98 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
+        <v>11</v>
+      </c>
+      <c r="B19" t="s">
         <v>12</v>
-      </c>
-      <c r="B19" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -1207,12 +1220,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C24"/>
+  <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1224,85 +1237,296 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="B1" s="8" t="s">
+    </row>
+    <row r="2" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+      <c r="A2" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B6" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B7" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B8" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="C1" s="8" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="72" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>64</v>
+    </row>
+    <row r="9" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B9" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B10" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B11" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B12" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B13" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B14" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B15" s="7" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="B16" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B17" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B18" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B19" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="22" spans="2:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B22" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="101.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>101</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="108.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="78.109375" customWidth="1"/>
+    <col min="3" max="3" width="26.6640625" style="2" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="C3" s="2" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>69</v>
-      </c>
       <c r="C4" s="2" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B6" s="2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B8" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B10" s="2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B12" s="2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B14" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B16" s="2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="18" spans="2:2" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B18" s="2" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="20" spans="2:2" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B20" s="2" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="22" spans="2:2" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B22" s="2" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B24" s="2" t="s">
-        <v>76</v>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B1" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="90.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>103</v>
       </c>
     </row>
   </sheetData>

</xml_diff>